<commit_message>
add variable names in tables
</commit_message>
<xml_diff>
--- a/7. Statistic Analysis/Datasheets/C/ManyBugs - C.xlsx
+++ b/7. Statistic Analysis/Datasheets/C/ManyBugs - C.xlsx
@@ -14,7 +14,94 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+  <si>
+    <t xml:space="preserve"><![CDATA[Var1]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Cyclomatic Complexity (CC)]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Maintainability Index]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbUnique Operands]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbOperands]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbUnique Operators]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbOperators]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Length]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Vocabulary Size]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Volume]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Difficulty Level]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Level]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[EffortTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[TimeTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NewVar5]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NewVar6]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Cyclomatic Complexity (CC)]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Maintainability Index]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbUnique Operands]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbOperands]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbUnique Operators]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[NbOperators]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Length]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Vocabulary Size]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Volume]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Difficulty Level]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[Program Level]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[EffortTo Implement]]></t>
+  </si>
+  <si>
+    <t xml:space="preserve"><![CDATA[TimeTo Implement]]></t>
+  </si>
   <si>
     <t xml:space="preserve"><![CDATA[angelix-gzip-884ef-fixed]]></t>
   </si>
@@ -521,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC19"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -562,94 +649,94 @@
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="n" s="0">
-        <v>9.570000</v>
-      </c>
-      <c r="C1" t="n" s="0">
-        <v>72.290000</v>
-      </c>
-      <c r="D1" t="n" s="0">
-        <v>15.140000</v>
-      </c>
-      <c r="E1" t="n" s="0">
-        <v>28.860000</v>
-      </c>
-      <c r="F1" t="n" s="0">
-        <v>8.860000</v>
-      </c>
-      <c r="G1" t="n" s="0">
-        <v>37.710000</v>
-      </c>
-      <c r="H1" t="n" s="0">
-        <v>66.570000</v>
-      </c>
-      <c r="I1" t="n" s="0">
-        <v>24.000000</v>
-      </c>
-      <c r="J1" t="n" s="0">
-        <v>393.810000</v>
-      </c>
-      <c r="K1" t="n" s="0">
-        <v>6.570000</v>
-      </c>
-      <c r="L1" t="n" s="0">
-        <v>0.230000</v>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="0">
+        <v>11</v>
       </c>
       <c r="M1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="N1" t="n" s="0">
-        <v>447.910000</v>
-      </c>
-      <c r="O1" t="n" s="0">
-        <v/>
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s" s="0">
+        <v>14</v>
       </c>
       <c r="P1" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="Q1" t="n" s="0">
-        <v>9.570000</v>
-      </c>
-      <c r="R1" t="n" s="0">
-        <v>72.290000</v>
-      </c>
-      <c r="S1" t="n" s="0">
-        <v>15.290000</v>
-      </c>
-      <c r="T1" t="n" s="0">
-        <v>29.140000</v>
-      </c>
-      <c r="U1" t="n" s="0">
-        <v>9.000000</v>
-      </c>
-      <c r="V1" t="n" s="0">
-        <v>38.140000</v>
-      </c>
-      <c r="W1" t="n" s="0">
-        <v>67.290000</v>
-      </c>
-      <c r="X1" t="n" s="0">
-        <v>24.290000</v>
-      </c>
-      <c r="Y1" t="n" s="0">
-        <v>399.970000</v>
-      </c>
-      <c r="Z1" t="n" s="0">
-        <v>6.860000</v>
-      </c>
-      <c r="AA1" t="n" s="0">
-        <v>0.230000</v>
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="AB1" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="AC1" t="n" s="0">
-        <v>491.180000</v>
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n" s="0">
         <v>9.570000</v>
@@ -685,7 +772,7 @@
         <v>0.230000</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="N2" t="n" s="0">
         <v>447.910000</v>
@@ -694,674 +781,674 @@
         <v/>
       </c>
       <c r="P2" t="s" s="0">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="Q2" t="n" s="0">
-        <v>9.710000</v>
+        <v>9.570000</v>
       </c>
       <c r="R2" t="n" s="0">
         <v>72.290000</v>
       </c>
       <c r="S2" t="n" s="0">
-        <v>15.430000</v>
+        <v>15.290000</v>
       </c>
       <c r="T2" t="n" s="0">
-        <v>29.290000</v>
+        <v>29.140000</v>
       </c>
       <c r="U2" t="n" s="0">
-        <v>8.860000</v>
+        <v>9.000000</v>
       </c>
       <c r="V2" t="n" s="0">
-        <v>38.570000</v>
+        <v>38.140000</v>
       </c>
       <c r="W2" t="n" s="0">
-        <v>67.860000</v>
+        <v>67.290000</v>
       </c>
       <c r="X2" t="n" s="0">
         <v>24.290000</v>
       </c>
       <c r="Y2" t="n" s="0">
-        <v>403.710000</v>
+        <v>399.970000</v>
       </c>
       <c r="Z2" t="n" s="0">
-        <v>6.570000</v>
+        <v>6.860000</v>
       </c>
       <c r="AA2" t="n" s="0">
         <v>0.230000</v>
       </c>
       <c r="AB2" t="s" s="0">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="AC2" t="n" s="0">
-        <v>461.110000</v>
+        <v>491.180000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>5.420000</v>
+        <v>9.570000</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>69.060000</v>
+        <v>72.290000</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>17.030000</v>
+        <v>15.140000</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>39.140000</v>
+        <v>28.860000</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>7.400000</v>
+        <v>8.860000</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>39.700000</v>
+        <v>37.710000</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>78.840000</v>
+        <v>66.570000</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>24.430000</v>
+        <v>24.000000</v>
       </c>
       <c r="J3" t="n" s="0">
-        <v>436.880000</v>
+        <v>393.810000</v>
       </c>
       <c r="K3" t="n" s="0">
-        <v>6.540000</v>
+        <v>6.570000</v>
       </c>
       <c r="L3" t="n" s="0">
-        <v>0.150000</v>
+        <v>0.230000</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="N3" t="n" s="0">
-        <v>513.530000</v>
+        <v>447.910000</v>
       </c>
       <c r="O3" t="n" s="0">
         <v/>
       </c>
       <c r="P3" t="s" s="0">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="Q3" t="n" s="0">
-        <v>5.420000</v>
+        <v>9.710000</v>
       </c>
       <c r="R3" t="n" s="0">
-        <v>69.060000</v>
+        <v>72.290000</v>
       </c>
       <c r="S3" t="n" s="0">
-        <v>17.030000</v>
+        <v>15.430000</v>
       </c>
       <c r="T3" t="n" s="0">
-        <v>39.140000</v>
+        <v>29.290000</v>
       </c>
       <c r="U3" t="n" s="0">
-        <v>7.400000</v>
+        <v>8.860000</v>
       </c>
       <c r="V3" t="n" s="0">
-        <v>39.700000</v>
+        <v>38.570000</v>
       </c>
       <c r="W3" t="n" s="0">
-        <v>78.840000</v>
+        <v>67.860000</v>
       </c>
       <c r="X3" t="n" s="0">
-        <v>24.430000</v>
+        <v>24.290000</v>
       </c>
       <c r="Y3" t="n" s="0">
-        <v>436.880000</v>
+        <v>403.710000</v>
       </c>
       <c r="Z3" t="n" s="0">
-        <v>6.540000</v>
+        <v>6.570000</v>
       </c>
       <c r="AA3" t="n" s="0">
-        <v>0.150000</v>
+        <v>0.230000</v>
       </c>
       <c r="AB3" t="s" s="0">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="AC3" t="n" s="0">
-        <v>513.530000</v>
+        <v>461.110000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>5.260000</v>
+        <v>5.420000</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>69.780000</v>
+        <v>69.060000</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>10.480000</v>
+        <v>17.030000</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>18.220000</v>
+        <v>39.140000</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>7.040000</v>
+        <v>7.400000</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>26.000000</v>
+        <v>39.700000</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>44.220000</v>
+        <v>78.840000</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>17.520000</v>
+        <v>24.430000</v>
       </c>
       <c r="J4" t="n" s="0">
-        <v>199.620000</v>
+        <v>436.880000</v>
       </c>
       <c r="K4" t="n" s="0">
-        <v>3.740000</v>
+        <v>6.540000</v>
       </c>
       <c r="L4" t="n" s="0">
-        <v>0.360000</v>
+        <v>0.150000</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="N4" t="n" s="0">
-        <v>82.830000</v>
+        <v>513.530000</v>
       </c>
       <c r="O4" t="n" s="0">
         <v/>
       </c>
       <c r="P4" t="s" s="0">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="Q4" t="n" s="0">
-        <v>5.260000</v>
+        <v>5.420000</v>
       </c>
       <c r="R4" t="n" s="0">
-        <v>69.780000</v>
+        <v>69.060000</v>
       </c>
       <c r="S4" t="n" s="0">
-        <v>10.480000</v>
+        <v>17.030000</v>
       </c>
       <c r="T4" t="n" s="0">
-        <v>18.220000</v>
+        <v>39.140000</v>
       </c>
       <c r="U4" t="n" s="0">
-        <v>7.040000</v>
+        <v>7.400000</v>
       </c>
       <c r="V4" t="n" s="0">
-        <v>26.000000</v>
+        <v>39.700000</v>
       </c>
       <c r="W4" t="n" s="0">
-        <v>44.220000</v>
+        <v>78.840000</v>
       </c>
       <c r="X4" t="n" s="0">
-        <v>17.520000</v>
+        <v>24.430000</v>
       </c>
       <c r="Y4" t="n" s="0">
-        <v>199.620000</v>
+        <v>436.880000</v>
       </c>
       <c r="Z4" t="n" s="0">
-        <v>3.740000</v>
+        <v>6.540000</v>
       </c>
       <c r="AA4" t="n" s="0">
-        <v>0.360000</v>
+        <v>0.150000</v>
       </c>
       <c r="AB4" t="s" s="0">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="AC4" t="n" s="0">
-        <v>82.830000</v>
+        <v>513.530000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>4.270000</v>
+        <v>5.260000</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>78.920000</v>
+        <v>69.780000</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>11.140000</v>
+        <v>10.480000</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>21.640000</v>
+        <v>18.220000</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>5.350000</v>
+        <v>7.040000</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>19.740000</v>
+        <v>26.000000</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>41.380000</v>
+        <v>44.220000</v>
       </c>
       <c r="I5" t="n" s="0">
-        <v>16.490000</v>
+        <v>17.520000</v>
       </c>
       <c r="J5" t="n" s="0">
-        <v>179.010000</v>
+        <v>199.620000</v>
       </c>
       <c r="K5" t="n" s="0">
-        <v>3.660000</v>
+        <v>3.740000</v>
       </c>
       <c r="L5" t="n" s="0">
-        <v>0.370000</v>
+        <v>0.360000</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="N5" t="n" s="0">
-        <v>61.200000</v>
+        <v>82.830000</v>
       </c>
       <c r="O5" t="n" s="0">
         <v/>
       </c>
       <c r="P5" t="s" s="0">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="Q5" t="n" s="0">
-        <v>4.270000</v>
+        <v>5.260000</v>
       </c>
       <c r="R5" t="n" s="0">
-        <v>78.920000</v>
+        <v>69.780000</v>
       </c>
       <c r="S5" t="n" s="0">
-        <v>11.160000</v>
+        <v>10.480000</v>
       </c>
       <c r="T5" t="n" s="0">
-        <v>21.660000</v>
+        <v>18.220000</v>
       </c>
       <c r="U5" t="n" s="0">
-        <v>5.350000</v>
+        <v>7.040000</v>
       </c>
       <c r="V5" t="n" s="0">
-        <v>19.750000</v>
+        <v>26.000000</v>
       </c>
       <c r="W5" t="n" s="0">
-        <v>41.420000</v>
+        <v>44.220000</v>
       </c>
       <c r="X5" t="n" s="0">
-        <v>16.510000</v>
+        <v>17.520000</v>
       </c>
       <c r="Y5" t="n" s="0">
-        <v>179.400000</v>
+        <v>199.620000</v>
       </c>
       <c r="Z5" t="n" s="0">
-        <v>3.660000</v>
+        <v>3.740000</v>
       </c>
       <c r="AA5" t="n" s="0">
-        <v>0.370000</v>
+        <v>0.360000</v>
       </c>
       <c r="AB5" t="s" s="0">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="AC5" t="n" s="0">
-        <v>61.500000</v>
+        <v>82.830000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>7.750000</v>
+        <v>4.270000</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>74.500000</v>
+        <v>78.920000</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>12.880000</v>
+        <v>11.140000</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>20.380000</v>
+        <v>21.640000</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>6.120000</v>
+        <v>5.350000</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>28.000000</v>
+        <v>19.740000</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>48.380000</v>
+        <v>41.380000</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>19.000000</v>
+        <v>16.490000</v>
       </c>
       <c r="J6" t="n" s="0">
-        <v>266.760000</v>
+        <v>179.010000</v>
       </c>
       <c r="K6" t="n" s="0">
-        <v>3.250000</v>
+        <v>3.660000</v>
       </c>
       <c r="L6" t="n" s="0">
         <v>0.370000</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="N6" t="n" s="0">
-        <v>115.310000</v>
+        <v>61.200000</v>
       </c>
       <c r="O6" t="n" s="0">
         <v/>
       </c>
       <c r="P6" t="s" s="0">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="Q6" t="n" s="0">
-        <v>7.750000</v>
+        <v>4.270000</v>
       </c>
       <c r="R6" t="n" s="0">
-        <v>74.500000</v>
+        <v>78.920000</v>
       </c>
       <c r="S6" t="n" s="0">
-        <v>12.880000</v>
+        <v>11.160000</v>
       </c>
       <c r="T6" t="n" s="0">
-        <v>20.380000</v>
+        <v>21.660000</v>
       </c>
       <c r="U6" t="n" s="0">
-        <v>6.120000</v>
+        <v>5.350000</v>
       </c>
       <c r="V6" t="n" s="0">
-        <v>28.000000</v>
+        <v>19.750000</v>
       </c>
       <c r="W6" t="n" s="0">
-        <v>48.380000</v>
+        <v>41.420000</v>
       </c>
       <c r="X6" t="n" s="0">
-        <v>19.000000</v>
+        <v>16.510000</v>
       </c>
       <c r="Y6" t="n" s="0">
-        <v>266.760000</v>
+        <v>179.400000</v>
       </c>
       <c r="Z6" t="n" s="0">
-        <v>3.250000</v>
+        <v>3.660000</v>
       </c>
       <c r="AA6" t="n" s="0">
         <v>0.370000</v>
       </c>
       <c r="AB6" t="s" s="0">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="AC6" t="n" s="0">
-        <v>115.310000</v>
+        <v>61.500000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B7" t="n" s="0">
-        <v>2.500000</v>
+        <v>7.750000</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>80.000000</v>
+        <v>74.500000</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>6.500000</v>
+        <v>12.880000</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>11.170000</v>
+        <v>20.380000</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>6.170000</v>
+        <v>6.120000</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>11.170000</v>
+        <v>28.000000</v>
       </c>
       <c r="H7" t="n" s="0">
-        <v>22.330000</v>
+        <v>48.380000</v>
       </c>
       <c r="I7" t="n" s="0">
-        <v>12.670000</v>
+        <v>19.000000</v>
       </c>
       <c r="J7" t="n" s="0">
-        <v>98.480000</v>
+        <v>266.760000</v>
       </c>
       <c r="K7" t="n" s="0">
-        <v>3.670000</v>
+        <v>3.250000</v>
       </c>
       <c r="L7" t="n" s="0">
-        <v>0.260000</v>
-      </c>
-      <c r="M7" t="n" s="0">
-        <v>742.820000</v>
+        <v>0.370000</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>50</v>
       </c>
       <c r="N7" t="n" s="0">
-        <v>41.270000</v>
+        <v>115.310000</v>
       </c>
       <c r="O7" t="n" s="0">
         <v/>
       </c>
       <c r="P7" t="s" s="0">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="Q7" t="n" s="0">
-        <v>2.500000</v>
+        <v>7.750000</v>
       </c>
       <c r="R7" t="n" s="0">
-        <v>80.000000</v>
+        <v>74.500000</v>
       </c>
       <c r="S7" t="n" s="0">
-        <v>6.500000</v>
+        <v>12.880000</v>
       </c>
       <c r="T7" t="n" s="0">
-        <v>11.170000</v>
+        <v>20.380000</v>
       </c>
       <c r="U7" t="n" s="0">
-        <v>6.170000</v>
+        <v>6.120000</v>
       </c>
       <c r="V7" t="n" s="0">
-        <v>11.170000</v>
+        <v>28.000000</v>
       </c>
       <c r="W7" t="n" s="0">
-        <v>22.330000</v>
+        <v>48.380000</v>
       </c>
       <c r="X7" t="n" s="0">
-        <v>12.670000</v>
+        <v>19.000000</v>
       </c>
       <c r="Y7" t="n" s="0">
-        <v>98.480000</v>
+        <v>266.760000</v>
       </c>
       <c r="Z7" t="n" s="0">
-        <v>3.670000</v>
+        <v>3.250000</v>
       </c>
       <c r="AA7" t="n" s="0">
-        <v>0.260000</v>
-      </c>
-      <c r="AB7" t="n" s="0">
-        <v>742.820000</v>
+        <v>0.370000</v>
+      </c>
+      <c r="AB7" t="s" s="0">
+        <v>52</v>
       </c>
       <c r="AC7" t="n" s="0">
-        <v>41.270000</v>
+        <v>115.310000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B8" t="n" s="0">
-        <v>5.420000</v>
+        <v>2.500000</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>69.060000</v>
+        <v>80.000000</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>17.030000</v>
+        <v>6.500000</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>39.140000</v>
+        <v>11.170000</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>7.400000</v>
+        <v>6.170000</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>39.700000</v>
+        <v>11.170000</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>78.840000</v>
+        <v>22.330000</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>24.430000</v>
+        <v>12.670000</v>
       </c>
       <c r="J8" t="n" s="0">
-        <v>436.880000</v>
+        <v>98.480000</v>
       </c>
       <c r="K8" t="n" s="0">
-        <v>6.540000</v>
+        <v>3.670000</v>
       </c>
       <c r="L8" t="n" s="0">
-        <v>0.150000</v>
-      </c>
-      <c r="M8" t="s" s="0">
-        <v>27</v>
+        <v>0.260000</v>
+      </c>
+      <c r="M8" t="n" s="0">
+        <v>742.820000</v>
       </c>
       <c r="N8" t="n" s="0">
-        <v>513.530000</v>
+        <v>41.270000</v>
       </c>
       <c r="O8" t="n" s="0">
         <v/>
       </c>
       <c r="P8" t="s" s="0">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="Q8" t="n" s="0">
-        <v>5.420000</v>
+        <v>2.500000</v>
       </c>
       <c r="R8" t="n" s="0">
-        <v>69.060000</v>
+        <v>80.000000</v>
       </c>
       <c r="S8" t="n" s="0">
-        <v>17.030000</v>
+        <v>6.500000</v>
       </c>
       <c r="T8" t="n" s="0">
-        <v>39.150000</v>
+        <v>11.170000</v>
       </c>
       <c r="U8" t="n" s="0">
-        <v>7.410000</v>
+        <v>6.170000</v>
       </c>
       <c r="V8" t="n" s="0">
-        <v>39.720000</v>
+        <v>11.170000</v>
       </c>
       <c r="W8" t="n" s="0">
-        <v>78.870000</v>
+        <v>22.330000</v>
       </c>
       <c r="X8" t="n" s="0">
-        <v>24.440000</v>
+        <v>12.670000</v>
       </c>
       <c r="Y8" t="n" s="0">
-        <v>437.170000</v>
+        <v>98.480000</v>
       </c>
       <c r="Z8" t="n" s="0">
-        <v>6.540000</v>
+        <v>3.670000</v>
       </c>
       <c r="AA8" t="n" s="0">
-        <v>0.150000</v>
-      </c>
-      <c r="AB8" t="s" s="0">
-        <v>29</v>
+        <v>0.260000</v>
+      </c>
+      <c r="AB8" t="n" s="0">
+        <v>742.820000</v>
       </c>
       <c r="AC8" t="n" s="0">
-        <v>514.010000</v>
+        <v>41.270000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>4.270000</v>
+        <v>5.420000</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>78.920000</v>
+        <v>69.060000</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>11.140000</v>
+        <v>17.030000</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>21.640000</v>
+        <v>39.140000</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>5.350000</v>
+        <v>7.400000</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>19.740000</v>
+        <v>39.700000</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>41.380000</v>
+        <v>78.840000</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>16.490000</v>
+        <v>24.430000</v>
       </c>
       <c r="J9" t="n" s="0">
-        <v>179.010000</v>
+        <v>436.880000</v>
       </c>
       <c r="K9" t="n" s="0">
-        <v>3.660000</v>
+        <v>6.540000</v>
       </c>
       <c r="L9" t="n" s="0">
-        <v>0.370000</v>
+        <v>0.150000</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="N9" t="n" s="0">
-        <v>61.200000</v>
+        <v>513.530000</v>
       </c>
       <c r="O9" t="n" s="0">
         <v/>
       </c>
       <c r="P9" t="s" s="0">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="Q9" t="n" s="0">
-        <v>4.270000</v>
+        <v>5.420000</v>
       </c>
       <c r="R9" t="n" s="0">
-        <v>78.920000</v>
+        <v>69.060000</v>
       </c>
       <c r="S9" t="n" s="0">
-        <v>11.160000</v>
+        <v>17.030000</v>
       </c>
       <c r="T9" t="n" s="0">
-        <v>21.660000</v>
+        <v>39.150000</v>
       </c>
       <c r="U9" t="n" s="0">
-        <v>5.350000</v>
+        <v>7.410000</v>
       </c>
       <c r="V9" t="n" s="0">
-        <v>19.750000</v>
+        <v>39.720000</v>
       </c>
       <c r="W9" t="n" s="0">
-        <v>41.420000</v>
+        <v>78.870000</v>
       </c>
       <c r="X9" t="n" s="0">
-        <v>16.510000</v>
+        <v>24.440000</v>
       </c>
       <c r="Y9" t="n" s="0">
-        <v>179.400000</v>
+        <v>437.170000</v>
       </c>
       <c r="Z9" t="n" s="0">
-        <v>3.660000</v>
+        <v>6.540000</v>
       </c>
       <c r="AA9" t="n" s="0">
-        <v>0.370000</v>
+        <v>0.150000</v>
       </c>
       <c r="AB9" t="s" s="0">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="AC9" t="n" s="0">
-        <v>61.500000</v>
+        <v>514.010000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B10" t="n" s="0">
         <v>4.270000</v>
@@ -1397,7 +1484,7 @@
         <v>0.370000</v>
       </c>
       <c r="M10" t="s" s="0">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="N10" t="n" s="0">
         <v>61.200000</v>
@@ -1406,10 +1493,10 @@
         <v/>
       </c>
       <c r="P10" t="s" s="0">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="Q10" t="n" s="0">
-        <v>4.290000</v>
+        <v>4.270000</v>
       </c>
       <c r="R10" t="n" s="0">
         <v>78.920000</v>
@@ -1418,22 +1505,22 @@
         <v>11.160000</v>
       </c>
       <c r="T10" t="n" s="0">
-        <v>21.680000</v>
+        <v>21.660000</v>
       </c>
       <c r="U10" t="n" s="0">
         <v>5.350000</v>
       </c>
       <c r="V10" t="n" s="0">
-        <v>19.780000</v>
+        <v>19.750000</v>
       </c>
       <c r="W10" t="n" s="0">
-        <v>41.450000</v>
+        <v>41.420000</v>
       </c>
       <c r="X10" t="n" s="0">
         <v>16.510000</v>
       </c>
       <c r="Y10" t="n" s="0">
-        <v>179.600000</v>
+        <v>179.400000</v>
       </c>
       <c r="Z10" t="n" s="0">
         <v>3.660000</v>
@@ -1442,810 +1529,899 @@
         <v>0.370000</v>
       </c>
       <c r="AB10" t="s" s="0">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="AC10" t="n" s="0">
-        <v>61.660000</v>
+        <v>61.500000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B11" t="n" s="0">
-        <v>2.330000</v>
+        <v>4.270000</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>81.000000</v>
+        <v>78.920000</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>7.000000</v>
+        <v>11.140000</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>14.670000</v>
+        <v>21.640000</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>5.330000</v>
+        <v>5.350000</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>9.670000</v>
+        <v>19.740000</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>24.330000</v>
+        <v>41.380000</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>12.330000</v>
+        <v>16.490000</v>
       </c>
       <c r="J11" t="n" s="0">
-        <v>109.000000</v>
+        <v>179.010000</v>
       </c>
       <c r="K11" t="n" s="0">
-        <v>4.000000</v>
+        <v>3.660000</v>
       </c>
       <c r="L11" t="n" s="0">
-        <v>0.200000</v>
-      </c>
-      <c r="M11" t="n" s="0">
-        <v>970.070000</v>
+        <v>0.370000</v>
+      </c>
+      <c r="M11" t="s" s="0">
+        <v>64</v>
       </c>
       <c r="N11" t="n" s="0">
-        <v>53.890000</v>
+        <v>61.200000</v>
       </c>
       <c r="O11" t="n" s="0">
         <v/>
       </c>
       <c r="P11" t="s" s="0">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="Q11" t="n" s="0">
-        <v>2.330000</v>
+        <v>4.290000</v>
       </c>
       <c r="R11" t="n" s="0">
-        <v>80.670000</v>
+        <v>78.920000</v>
       </c>
       <c r="S11" t="n" s="0">
-        <v>7.670000</v>
+        <v>11.160000</v>
       </c>
       <c r="T11" t="n" s="0">
-        <v>15.330000</v>
+        <v>21.680000</v>
       </c>
       <c r="U11" t="n" s="0">
-        <v>5.670000</v>
+        <v>5.350000</v>
       </c>
       <c r="V11" t="n" s="0">
-        <v>10.000000</v>
+        <v>19.780000</v>
       </c>
       <c r="W11" t="n" s="0">
-        <v>25.330000</v>
+        <v>41.450000</v>
       </c>
       <c r="X11" t="n" s="0">
-        <v>13.330000</v>
+        <v>16.510000</v>
       </c>
       <c r="Y11" t="n" s="0">
-        <v>114.310000</v>
+        <v>179.600000</v>
       </c>
       <c r="Z11" t="n" s="0">
-        <v>4.330000</v>
+        <v>3.660000</v>
       </c>
       <c r="AA11" t="n" s="0">
-        <v>0.140000</v>
+        <v>0.370000</v>
       </c>
       <c r="AB11" t="s" s="0">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="AC11" t="n" s="0">
-        <v>55.610000</v>
+        <v>61.660000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B12" t="n" s="0">
-        <v>5.250000</v>
+        <v>2.330000</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>77.000000</v>
+        <v>81.000000</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>7.750000</v>
+        <v>7.000000</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>13.000000</v>
+        <v>14.670000</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>3.500000</v>
+        <v>5.330000</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>17.000000</v>
+        <v>9.670000</v>
       </c>
       <c r="H12" t="n" s="0">
-        <v>30.000000</v>
+        <v>24.330000</v>
       </c>
       <c r="I12" t="n" s="0">
-        <v>11.250000</v>
+        <v>12.330000</v>
       </c>
       <c r="J12" t="n" s="0">
-        <v>125.930000</v>
+        <v>109.000000</v>
       </c>
       <c r="K12" t="n" s="0">
-        <v>1.500000</v>
+        <v>4.000000</v>
       </c>
       <c r="L12" t="n" s="0">
-        <v>0.460000</v>
+        <v>0.200000</v>
       </c>
       <c r="M12" t="n" s="0">
-        <v>282.010000</v>
+        <v>970.070000</v>
       </c>
       <c r="N12" t="n" s="0">
-        <v>15.670000</v>
+        <v>53.890000</v>
       </c>
       <c r="O12" t="n" s="0">
         <v/>
       </c>
       <c r="P12" t="s" s="0">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="Q12" t="n" s="0">
-        <v>5.250000</v>
+        <v>2.330000</v>
       </c>
       <c r="R12" t="n" s="0">
-        <v>77.000000</v>
+        <v>80.670000</v>
       </c>
       <c r="S12" t="n" s="0">
-        <v>7.750000</v>
+        <v>7.670000</v>
       </c>
       <c r="T12" t="n" s="0">
-        <v>13.000000</v>
+        <v>15.330000</v>
       </c>
       <c r="U12" t="n" s="0">
-        <v>3.500000</v>
+        <v>5.670000</v>
       </c>
       <c r="V12" t="n" s="0">
-        <v>17.000000</v>
+        <v>10.000000</v>
       </c>
       <c r="W12" t="n" s="0">
-        <v>30.000000</v>
+        <v>25.330000</v>
       </c>
       <c r="X12" t="n" s="0">
-        <v>11.250000</v>
+        <v>13.330000</v>
       </c>
       <c r="Y12" t="n" s="0">
-        <v>125.930000</v>
+        <v>114.310000</v>
       </c>
       <c r="Z12" t="n" s="0">
-        <v>1.500000</v>
+        <v>4.330000</v>
       </c>
       <c r="AA12" t="n" s="0">
-        <v>0.460000</v>
-      </c>
-      <c r="AB12" t="n" s="0">
-        <v>282.010000</v>
+        <v>0.140000</v>
+      </c>
+      <c r="AB12" t="s" s="0">
+        <v>69</v>
       </c>
       <c r="AC12" t="n" s="0">
-        <v>15.670000</v>
+        <v>55.610000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B13" t="n" s="0">
-        <v>2.670000</v>
+        <v>5.250000</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>88.330000</v>
+        <v>77.000000</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>4.000000</v>
+        <v>7.750000</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>5.670000</v>
+        <v>13.000000</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>2.000000</v>
+        <v>3.500000</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>8.000000</v>
+        <v>17.000000</v>
       </c>
       <c r="H13" t="n" s="0">
-        <v>13.670000</v>
+        <v>30.000000</v>
       </c>
       <c r="I13" t="n" s="0">
-        <v>6.000000</v>
+        <v>11.250000</v>
       </c>
       <c r="J13" t="n" s="0">
-        <v>48.280000</v>
+        <v>125.930000</v>
       </c>
       <c r="K13" t="n" s="0">
-        <v>0.670000</v>
+        <v>1.500000</v>
       </c>
       <c r="L13" t="n" s="0">
-        <v>0.170000</v>
+        <v>0.460000</v>
       </c>
       <c r="M13" t="n" s="0">
-        <v>88.810000</v>
+        <v>282.010000</v>
       </c>
       <c r="N13" t="n" s="0">
-        <v>4.930000</v>
+        <v>15.670000</v>
       </c>
       <c r="O13" t="n" s="0">
         <v/>
       </c>
       <c r="P13" t="s" s="0">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="Q13" t="n" s="0">
-        <v>2.670000</v>
+        <v>5.250000</v>
       </c>
       <c r="R13" t="n" s="0">
-        <v>88.330000</v>
+        <v>77.000000</v>
       </c>
       <c r="S13" t="n" s="0">
-        <v>4.000000</v>
+        <v>7.750000</v>
       </c>
       <c r="T13" t="n" s="0">
-        <v>5.670000</v>
+        <v>13.000000</v>
       </c>
       <c r="U13" t="n" s="0">
-        <v>2.000000</v>
+        <v>3.500000</v>
       </c>
       <c r="V13" t="n" s="0">
-        <v>8.000000</v>
+        <v>17.000000</v>
       </c>
       <c r="W13" t="n" s="0">
-        <v>13.670000</v>
+        <v>30.000000</v>
       </c>
       <c r="X13" t="n" s="0">
-        <v>6.000000</v>
+        <v>11.250000</v>
       </c>
       <c r="Y13" t="n" s="0">
-        <v>48.280000</v>
+        <v>125.930000</v>
       </c>
       <c r="Z13" t="n" s="0">
-        <v>0.670000</v>
+        <v>1.500000</v>
       </c>
       <c r="AA13" t="n" s="0">
-        <v>0.170000</v>
+        <v>0.460000</v>
       </c>
       <c r="AB13" t="n" s="0">
-        <v>88.810000</v>
+        <v>282.010000</v>
       </c>
       <c r="AC13" t="n" s="0">
-        <v>4.930000</v>
+        <v>15.670000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B14" t="n" s="0">
-        <v>1.000000</v>
+        <v>2.670000</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>100.000000</v>
+        <v>88.330000</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>0.000000</v>
+        <v>4.000000</v>
       </c>
       <c r="E14" t="n" s="0">
-        <v>0.000000</v>
+        <v>5.670000</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>0.000000</v>
+        <v>2.000000</v>
       </c>
       <c r="G14" t="n" s="0">
-        <v>0.000000</v>
+        <v>8.000000</v>
       </c>
       <c r="H14" t="n" s="0">
-        <v>0.000000</v>
+        <v>13.670000</v>
       </c>
       <c r="I14" t="n" s="0">
-        <v>0.000000</v>
+        <v>6.000000</v>
       </c>
       <c r="J14" t="n" s="0">
-        <v>0.000000</v>
+        <v>48.280000</v>
       </c>
       <c r="K14" t="n" s="0">
-        <v>0.000000</v>
+        <v>0.670000</v>
       </c>
       <c r="L14" t="n" s="0">
-        <v>0.000000</v>
+        <v>0.170000</v>
       </c>
       <c r="M14" t="n" s="0">
-        <v>0.000000</v>
+        <v>88.810000</v>
       </c>
       <c r="N14" t="n" s="0">
-        <v>0.000000</v>
+        <v>4.930000</v>
       </c>
       <c r="O14" t="n" s="0">
         <v/>
       </c>
       <c r="P14" t="s" s="0">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="Q14" t="n" s="0">
-        <v>1.000000</v>
+        <v>2.670000</v>
       </c>
       <c r="R14" t="n" s="0">
-        <v>100.000000</v>
+        <v>88.330000</v>
       </c>
       <c r="S14" t="n" s="0">
-        <v>0.000000</v>
+        <v>4.000000</v>
       </c>
       <c r="T14" t="n" s="0">
-        <v>0.000000</v>
+        <v>5.670000</v>
       </c>
       <c r="U14" t="n" s="0">
-        <v>0.000000</v>
+        <v>2.000000</v>
       </c>
       <c r="V14" t="n" s="0">
-        <v>0.000000</v>
+        <v>8.000000</v>
       </c>
       <c r="W14" t="n" s="0">
-        <v>0.000000</v>
+        <v>13.670000</v>
       </c>
       <c r="X14" t="n" s="0">
-        <v>0.000000</v>
+        <v>6.000000</v>
       </c>
       <c r="Y14" t="n" s="0">
-        <v>0.000000</v>
+        <v>48.280000</v>
       </c>
       <c r="Z14" t="n" s="0">
-        <v>0.000000</v>
+        <v>0.670000</v>
       </c>
       <c r="AA14" t="n" s="0">
-        <v>0.000000</v>
+        <v>0.170000</v>
       </c>
       <c r="AB14" t="n" s="0">
-        <v>0.000000</v>
+        <v>88.810000</v>
       </c>
       <c r="AC14" t="n" s="0">
-        <v>0.000000</v>
+        <v>4.930000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B15" t="n" s="0">
-        <v>5.000000</v>
+        <v>1.000000</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>76.860000</v>
+        <v>100.000000</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>8.430000</v>
+        <v>0.000000</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>13.140000</v>
+        <v>0.000000</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>5.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="G15" t="n" s="0">
-        <v>19.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="H15" t="n" s="0">
-        <v>32.430000</v>
+        <v>0.000000</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>13.710000</v>
+        <v>0.000000</v>
       </c>
       <c r="J15" t="n" s="0">
-        <v>139.900000</v>
+        <v>0.000000</v>
       </c>
       <c r="K15" t="n" s="0">
-        <v>3.430000</v>
+        <v>0.000000</v>
       </c>
       <c r="L15" t="n" s="0">
-        <v>0.460000</v>
+        <v>0.000000</v>
       </c>
       <c r="M15" t="n" s="0">
-        <v>916.650000</v>
+        <v>0.000000</v>
       </c>
       <c r="N15" t="n" s="0">
-        <v>50.930000</v>
+        <v>0.000000</v>
       </c>
       <c r="O15" t="n" s="0">
         <v/>
       </c>
       <c r="P15" t="s" s="0">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="Q15" t="n" s="0">
-        <v>5.140000</v>
+        <v>1.000000</v>
       </c>
       <c r="R15" t="n" s="0">
-        <v>76.290000</v>
+        <v>100.000000</v>
       </c>
       <c r="S15" t="n" s="0">
-        <v>9.140000</v>
+        <v>0.000000</v>
       </c>
       <c r="T15" t="n" s="0">
-        <v>15.570000</v>
+        <v>0.000000</v>
       </c>
       <c r="U15" t="n" s="0">
-        <v>6.140000</v>
+        <v>0.000000</v>
       </c>
       <c r="V15" t="n" s="0">
-        <v>22.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="W15" t="n" s="0">
-        <v>37.860000</v>
+        <v>0.000000</v>
       </c>
       <c r="X15" t="n" s="0">
-        <v>15.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="Y15" t="n" s="0">
-        <v>172.210000</v>
+        <v>0.000000</v>
       </c>
       <c r="Z15" t="n" s="0">
-        <v>4.000000</v>
+        <v>0.000000</v>
       </c>
       <c r="AA15" t="n" s="0">
-        <v>0.440000</v>
-      </c>
-      <c r="AB15" t="s" s="0">
-        <v>49</v>
+        <v>0.000000</v>
+      </c>
+      <c r="AB15" t="n" s="0">
+        <v>0.000000</v>
       </c>
       <c r="AC15" t="n" s="0">
-        <v>79.040000</v>
+        <v>0.000000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B16" t="n" s="0">
-        <v>1.000000</v>
+        <v>5.000000</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>100.000000</v>
+        <v>76.860000</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>0.000000</v>
+        <v>8.430000</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>0.000000</v>
+        <v>13.140000</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>0.000000</v>
+        <v>5.290000</v>
       </c>
       <c r="G16" t="n" s="0">
-        <v>0.000000</v>
+        <v>19.290000</v>
       </c>
       <c r="H16" t="n" s="0">
-        <v>0.000000</v>
+        <v>32.430000</v>
       </c>
       <c r="I16" t="n" s="0">
-        <v>0.000000</v>
+        <v>13.710000</v>
       </c>
       <c r="J16" t="n" s="0">
-        <v>0.000000</v>
+        <v>139.900000</v>
       </c>
       <c r="K16" t="n" s="0">
-        <v>0.000000</v>
+        <v>3.430000</v>
       </c>
       <c r="L16" t="n" s="0">
-        <v>0.000000</v>
+        <v>0.460000</v>
       </c>
       <c r="M16" t="n" s="0">
-        <v>0.000000</v>
+        <v>916.650000</v>
       </c>
       <c r="N16" t="n" s="0">
-        <v>0.000000</v>
+        <v>50.930000</v>
       </c>
       <c r="O16" t="n" s="0">
         <v/>
       </c>
       <c r="P16" t="s" s="0">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="Q16" t="n" s="0">
-        <v>1.000000</v>
+        <v>5.140000</v>
       </c>
       <c r="R16" t="n" s="0">
-        <v>100.000000</v>
+        <v>76.290000</v>
       </c>
       <c r="S16" t="n" s="0">
-        <v>0.000000</v>
+        <v>9.140000</v>
       </c>
       <c r="T16" t="n" s="0">
-        <v>0.000000</v>
+        <v>15.570000</v>
       </c>
       <c r="U16" t="n" s="0">
-        <v>0.000000</v>
+        <v>6.140000</v>
       </c>
       <c r="V16" t="n" s="0">
-        <v>0.000000</v>
+        <v>22.290000</v>
       </c>
       <c r="W16" t="n" s="0">
-        <v>0.000000</v>
+        <v>37.860000</v>
       </c>
       <c r="X16" t="n" s="0">
-        <v>0.000000</v>
+        <v>15.290000</v>
       </c>
       <c r="Y16" t="n" s="0">
-        <v>0.000000</v>
+        <v>172.210000</v>
       </c>
       <c r="Z16" t="n" s="0">
-        <v>0.000000</v>
+        <v>4.000000</v>
       </c>
       <c r="AA16" t="n" s="0">
-        <v>0.000000</v>
-      </c>
-      <c r="AB16" t="n" s="0">
-        <v>0.000000</v>
+        <v>0.440000</v>
+      </c>
+      <c r="AB16" t="s" s="0">
+        <v>78</v>
       </c>
       <c r="AC16" t="n" s="0">
-        <v>0.000000</v>
+        <v>79.040000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B17" t="n" s="0">
-        <v>2.070000</v>
+        <v>1.000000</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>88.290000</v>
+        <v>100.000000</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>4.860000</v>
+        <v>0.000000</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>6.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>3.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="G17" t="n" s="0">
-        <v>6.710000</v>
+        <v>0.000000</v>
       </c>
       <c r="H17" t="n" s="0">
-        <v>13.000000</v>
+        <v>0.000000</v>
       </c>
       <c r="I17" t="n" s="0">
-        <v>8.140000</v>
+        <v>0.000000</v>
       </c>
       <c r="J17" t="n" s="0">
-        <v>45.620000</v>
+        <v>0.000000</v>
       </c>
       <c r="K17" t="n" s="0">
-        <v>1.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="L17" t="n" s="0">
-        <v>0.640000</v>
+        <v>0.000000</v>
       </c>
       <c r="M17" t="n" s="0">
-        <v>120.500000</v>
+        <v>0.000000</v>
       </c>
       <c r="N17" t="n" s="0">
-        <v>6.690000</v>
+        <v>0.000000</v>
       </c>
       <c r="O17" t="n" s="0">
         <v/>
       </c>
       <c r="P17" t="s" s="0">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="Q17" t="n" s="0">
-        <v>2.070000</v>
+        <v>1.000000</v>
       </c>
       <c r="R17" t="n" s="0">
-        <v>88.290000</v>
+        <v>100.000000</v>
       </c>
       <c r="S17" t="n" s="0">
-        <v>4.860000</v>
+        <v>0.000000</v>
       </c>
       <c r="T17" t="n" s="0">
-        <v>6.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="U17" t="n" s="0">
-        <v>3.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="V17" t="n" s="0">
-        <v>6.710000</v>
+        <v>0.000000</v>
       </c>
       <c r="W17" t="n" s="0">
-        <v>13.000000</v>
+        <v>0.000000</v>
       </c>
       <c r="X17" t="n" s="0">
-        <v>8.140000</v>
+        <v>0.000000</v>
       </c>
       <c r="Y17" t="n" s="0">
-        <v>45.620000</v>
+        <v>0.000000</v>
       </c>
       <c r="Z17" t="n" s="0">
-        <v>1.290000</v>
+        <v>0.000000</v>
       </c>
       <c r="AA17" t="n" s="0">
-        <v>0.640000</v>
+        <v>0.000000</v>
       </c>
       <c r="AB17" t="n" s="0">
-        <v>120.500000</v>
+        <v>0.000000</v>
       </c>
       <c r="AC17" t="n" s="0">
-        <v>6.690000</v>
+        <v>0.000000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="B18" t="n" s="0">
-        <v>5.000000</v>
+        <v>2.070000</v>
       </c>
       <c r="C18" t="n" s="0">
-        <v>76.860000</v>
+        <v>88.290000</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>8.430000</v>
+        <v>4.860000</v>
       </c>
       <c r="E18" t="n" s="0">
-        <v>13.140000</v>
+        <v>6.290000</v>
       </c>
       <c r="F18" t="n" s="0">
-        <v>5.290000</v>
+        <v>3.290000</v>
       </c>
       <c r="G18" t="n" s="0">
-        <v>19.290000</v>
+        <v>6.710000</v>
       </c>
       <c r="H18" t="n" s="0">
-        <v>32.430000</v>
+        <v>13.000000</v>
       </c>
       <c r="I18" t="n" s="0">
-        <v>13.710000</v>
+        <v>8.140000</v>
       </c>
       <c r="J18" t="n" s="0">
-        <v>139.900000</v>
+        <v>45.620000</v>
       </c>
       <c r="K18" t="n" s="0">
-        <v>3.430000</v>
+        <v>1.290000</v>
       </c>
       <c r="L18" t="n" s="0">
-        <v>0.460000</v>
+        <v>0.640000</v>
       </c>
       <c r="M18" t="n" s="0">
-        <v>916.650000</v>
+        <v>120.500000</v>
       </c>
       <c r="N18" t="n" s="0">
-        <v>50.930000</v>
+        <v>6.690000</v>
       </c>
       <c r="O18" t="n" s="0">
         <v/>
       </c>
       <c r="P18" t="s" s="0">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="Q18" t="n" s="0">
-        <v>5.140000</v>
+        <v>2.070000</v>
       </c>
       <c r="R18" t="n" s="0">
-        <v>76.290000</v>
+        <v>88.290000</v>
       </c>
       <c r="S18" t="n" s="0">
-        <v>9.140000</v>
+        <v>4.860000</v>
       </c>
       <c r="T18" t="n" s="0">
-        <v>15.570000</v>
+        <v>6.290000</v>
       </c>
       <c r="U18" t="n" s="0">
-        <v>6.140000</v>
+        <v>3.290000</v>
       </c>
       <c r="V18" t="n" s="0">
-        <v>22.290000</v>
+        <v>6.710000</v>
       </c>
       <c r="W18" t="n" s="0">
-        <v>37.860000</v>
+        <v>13.000000</v>
       </c>
       <c r="X18" t="n" s="0">
-        <v>15.290000</v>
+        <v>8.140000</v>
       </c>
       <c r="Y18" t="n" s="0">
-        <v>172.210000</v>
+        <v>45.620000</v>
       </c>
       <c r="Z18" t="n" s="0">
-        <v>4.000000</v>
+        <v>1.290000</v>
       </c>
       <c r="AA18" t="n" s="0">
-        <v>0.440000</v>
-      </c>
-      <c r="AB18" t="s" s="0">
-        <v>56</v>
+        <v>0.640000</v>
+      </c>
+      <c r="AB18" t="n" s="0">
+        <v>120.500000</v>
       </c>
       <c r="AC18" t="n" s="0">
-        <v>79.040000</v>
+        <v>6.690000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B19" t="n" s="0">
-        <v>2.820000</v>
+        <v>5.000000</v>
       </c>
       <c r="C19" t="n" s="0">
-        <v>80.410000</v>
+        <v>76.860000</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>6.120000</v>
+        <v>8.430000</v>
       </c>
       <c r="E19" t="n" s="0">
-        <v>9.410000</v>
+        <v>13.140000</v>
       </c>
       <c r="F19" t="n" s="0">
-        <v>4.940000</v>
+        <v>5.290000</v>
       </c>
       <c r="G19" t="n" s="0">
-        <v>10.350000</v>
+        <v>19.290000</v>
       </c>
       <c r="H19" t="n" s="0">
-        <v>19.760000</v>
+        <v>32.430000</v>
       </c>
       <c r="I19" t="n" s="0">
-        <v>11.060000</v>
+        <v>13.710000</v>
       </c>
       <c r="J19" t="n" s="0">
-        <v>77.650000</v>
+        <v>139.900000</v>
       </c>
       <c r="K19" t="n" s="0">
-        <v>2.760000</v>
+        <v>3.430000</v>
       </c>
       <c r="L19" t="n" s="0">
-        <v>0.430000</v>
+        <v>0.460000</v>
       </c>
       <c r="M19" t="n" s="0">
-        <v>428.460000</v>
+        <v>916.650000</v>
       </c>
       <c r="N19" t="n" s="0">
-        <v>23.800000</v>
+        <v>50.930000</v>
       </c>
       <c r="O19" t="n" s="0">
         <v/>
       </c>
       <c r="P19" t="s" s="0">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="Q19" t="n" s="0">
+        <v>5.140000</v>
+      </c>
+      <c r="R19" t="n" s="0">
+        <v>76.290000</v>
+      </c>
+      <c r="S19" t="n" s="0">
+        <v>9.140000</v>
+      </c>
+      <c r="T19" t="n" s="0">
+        <v>15.570000</v>
+      </c>
+      <c r="U19" t="n" s="0">
+        <v>6.140000</v>
+      </c>
+      <c r="V19" t="n" s="0">
+        <v>22.290000</v>
+      </c>
+      <c r="W19" t="n" s="0">
+        <v>37.860000</v>
+      </c>
+      <c r="X19" t="n" s="0">
+        <v>15.290000</v>
+      </c>
+      <c r="Y19" t="n" s="0">
+        <v>172.210000</v>
+      </c>
+      <c r="Z19" t="n" s="0">
+        <v>4.000000</v>
+      </c>
+      <c r="AA19" t="n" s="0">
+        <v>0.440000</v>
+      </c>
+      <c r="AB19" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="AC19" t="n" s="0">
+        <v>79.040000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B20" t="n" s="0">
         <v>2.820000</v>
       </c>
-      <c r="R19" t="n" s="0">
+      <c r="C20" t="n" s="0">
+        <v>80.410000</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>6.120000</v>
+      </c>
+      <c r="E20" t="n" s="0">
+        <v>9.410000</v>
+      </c>
+      <c r="F20" t="n" s="0">
+        <v>4.940000</v>
+      </c>
+      <c r="G20" t="n" s="0">
+        <v>10.350000</v>
+      </c>
+      <c r="H20" t="n" s="0">
+        <v>19.760000</v>
+      </c>
+      <c r="I20" t="n" s="0">
+        <v>11.060000</v>
+      </c>
+      <c r="J20" t="n" s="0">
+        <v>77.650000</v>
+      </c>
+      <c r="K20" t="n" s="0">
+        <v>2.760000</v>
+      </c>
+      <c r="L20" t="n" s="0">
+        <v>0.430000</v>
+      </c>
+      <c r="M20" t="n" s="0">
+        <v>428.460000</v>
+      </c>
+      <c r="N20" t="n" s="0">
+        <v>23.800000</v>
+      </c>
+      <c r="O20" t="n" s="0">
+        <v/>
+      </c>
+      <c r="P20" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="Q20" t="n" s="0">
+        <v>2.820000</v>
+      </c>
+      <c r="R20" t="n" s="0">
         <v>80.710000</v>
       </c>
-      <c r="S19" t="n" s="0">
+      <c r="S20" t="n" s="0">
         <v>6.000000</v>
       </c>
-      <c r="T19" t="n" s="0">
+      <c r="T20" t="n" s="0">
         <v>9.120000</v>
       </c>
-      <c r="U19" t="n" s="0">
+      <c r="U20" t="n" s="0">
         <v>4.880000</v>
       </c>
-      <c r="V19" t="n" s="0">
+      <c r="V20" t="n" s="0">
         <v>10.180000</v>
       </c>
-      <c r="W19" t="n" s="0">
+      <c r="W20" t="n" s="0">
         <v>19.290000</v>
       </c>
-      <c r="X19" t="n" s="0">
+      <c r="X20" t="n" s="0">
         <v>10.880000</v>
       </c>
-      <c r="Y19" t="n" s="0">
+      <c r="Y20" t="n" s="0">
         <v>75.470000</v>
       </c>
-      <c r="Z19" t="n" s="0">
+      <c r="Z20" t="n" s="0">
         <v>2.760000</v>
       </c>
-      <c r="AA19" t="n" s="0">
+      <c r="AA20" t="n" s="0">
         <v>0.430000</v>
       </c>
-      <c r="AB19" t="n" s="0">
+      <c r="AB20" t="n" s="0">
         <v>421.910000</v>
       </c>
-      <c r="AC19" t="n" s="0">
+      <c r="AC20" t="n" s="0">
         <v>23.440000</v>
       </c>
     </row>

</xml_diff>